<commit_message>
random user agent & proxy supported & longman dictionary supported
</commit_message>
<xml_diff>
--- a/words2.xlsx
+++ b/words2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文件\word_recreation_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yyc\Desktop\Extracurricula Projects\dictionary-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6B447E-6FEB-47C2-8A89-5D86097B48DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7A6564-00F8-4B0C-BE6B-D4B807A6B591}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1131" yWindow="1131" windowWidth="17863" windowHeight="12240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="264">
   <si>
     <t>#带井号的不会统计</t>
   </si>
@@ -244,124 +244,767 @@
     <t>jywyes</t>
   </si>
   <si>
-    <t>displace</t>
-  </si>
-  <si>
-    <t>disposal</t>
-  </si>
-  <si>
-    <t>disposition</t>
-  </si>
-  <si>
-    <t>disregard</t>
-  </si>
-  <si>
-    <t>disrupt</t>
-  </si>
-  <si>
-    <t>dissipate</t>
-  </si>
-  <si>
-    <t>distill</t>
-  </si>
-  <si>
-    <t>distort</t>
-  </si>
-  <si>
-    <t>distract</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>disturbance</t>
-  </si>
-  <si>
-    <t>diversion</t>
-  </si>
-  <si>
-    <t>divert</t>
-  </si>
-  <si>
-    <t>divine</t>
-  </si>
-  <si>
-    <t>divorce</t>
-  </si>
-  <si>
-    <t>dizzy</t>
-  </si>
-  <si>
-    <t>dock</t>
-  </si>
-  <si>
-    <t>doctrine</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>dome</t>
-  </si>
-  <si>
-    <t>donate</t>
-  </si>
-  <si>
-    <t>doom</t>
-  </si>
-  <si>
-    <t>drag</t>
-  </si>
-  <si>
-    <t>drainage</t>
-  </si>
-  <si>
-    <t>dramatic</t>
-  </si>
-  <si>
-    <t>drastic</t>
-  </si>
-  <si>
-    <t>drawback</t>
-  </si>
-  <si>
-    <t>dread</t>
-  </si>
-  <si>
-    <t>drill</t>
-  </si>
-  <si>
-    <t>drought</t>
-  </si>
-  <si>
-    <t>dual</t>
-  </si>
-  <si>
-    <t>dubious</t>
-  </si>
-  <si>
-    <t>duration</t>
-  </si>
-  <si>
-    <t>dwell</t>
-  </si>
-  <si>
-    <t>earnings</t>
-  </si>
-  <si>
-    <t>ease</t>
-  </si>
-  <si>
-    <t>eccentric</t>
-  </si>
-  <si>
-    <t>eclipse</t>
-  </si>
-  <si>
-    <t>ecology</t>
-  </si>
-  <si>
     <t>#new</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cabbage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cabin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calendar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>camel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>camp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campaign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>can</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>canal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>candidate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>candle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>candy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>canteen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capital</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>captain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>car</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carbon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>card</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>care</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caeer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>careful</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>careless</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carriage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartoon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>casual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>catalogue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>catch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cause</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cease</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ceiling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>celebrate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>central</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>centre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>century</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ceremony</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>certain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>certificate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chairman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>challenge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>champion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chapter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>characteristic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>charge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>charity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>charm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chemical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheque</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chief</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>childish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>church</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>circular</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>circumstance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>citizen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>civil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>civilian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>claim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>climate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>club</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>college</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>combination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>combine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>come</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comfort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>command</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commerical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>communicate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>complex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>composition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comprehension</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compulsory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conceal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>concern</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>concrete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conduct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>congress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>consequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>consume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contract</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>convey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cope</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corporation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>correct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>could</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>couple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>course</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>court</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>craft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crawl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crazy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>credit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crisis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>critical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>criticize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crowd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crucial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crystal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cultivate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curtain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cycle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -439,7 +1082,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -447,9 +1090,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -738,9 +1378,9 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -786,7 +1426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -797,7 +1437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -805,7 +1445,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -813,7 +1453,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -824,7 +1464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -835,7 +1475,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -846,7 +1486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -857,7 +1497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -882,9 +1522,9 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +1541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -930,7 +1570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -938,7 +1578,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -946,7 +1586,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -954,7 +1594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -962,7 +1602,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -970,7 +1610,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -978,7 +1618,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -986,7 +1626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -994,7 +1634,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1002,7 +1642,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1010,7 +1650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -1018,7 +1658,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -1040,9 +1680,9 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1088,7 +1728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1099,7 +1739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1110,7 +1750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -1118,17 +1758,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1136,7 +1776,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1144,7 +1784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -1152,7 +1792,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -1160,7 +1800,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -1168,7 +1808,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1176,7 +1816,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1184,7 +1824,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1192,7 +1832,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1200,7 +1840,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1208,7 +1848,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1224,15 +1864,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A4" sqref="A4:A193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1281,205 +1921,960 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>111</v>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>